<commit_message>
final data (may still need filtering)
</commit_message>
<xml_diff>
--- a/reference/Data Format.xlsx
+++ b/reference/Data Format.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/victorperso/Documents/EUR/Aegon Marketing Case/baqm-seminar-16/reference/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBB4AAD4-0B57-6F44-939F-CC638BC0B05D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2652DB3-E97F-7E49-BBC5-0DAEE6F31949}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{A5F595FE-D205-7E44-A0CB-1A074940655C}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17180" xr2:uid="{A5F595FE-D205-7E44-A0CB-1A074940655C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -186,7 +186,7 @@
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="164" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="166" formatCode="_ * #,##0.000_ ;_ * \-#,##0.000_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="165" formatCode="_ * #,##0.000_ ;_ * \-#,##0.000_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -210,12 +210,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -232,19 +238,22 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -565,8 +574,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DB9708A-421A-0241-B3D4-7CDDEED0A0CB}">
   <dimension ref="B2:Y22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="158" workbookViewId="0">
+      <selection activeCell="I13" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -727,16 +736,36 @@
       <c r="I7" s="6"/>
     </row>
     <row r="8" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="C8" t="s">
+      <c r="B8" s="9"/>
+      <c r="C8" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="F8" t="s">
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="V8" s="9" t="s">
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
+      <c r="N8" s="9"/>
+      <c r="O8" s="9"/>
+      <c r="P8" s="9"/>
+      <c r="Q8" s="9"/>
+      <c r="R8" s="10"/>
+      <c r="S8" s="10"/>
+      <c r="T8" s="10"/>
+      <c r="U8" s="10"/>
+      <c r="V8" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="W8" s="9"/>
+      <c r="W8" s="12"/>
+      <c r="X8" s="11"/>
+      <c r="Y8" s="11"/>
     </row>
     <row r="9" spans="2:25" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
@@ -1027,6 +1056,7 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <ignoredErrors>
     <ignoredError sqref="X19:X22" formulaRange="1"/>
   </ignoredErrors>

</xml_diff>